<commit_message>
21-06-16 Preprocessing, Modeling Practice
</commit_message>
<xml_diff>
--- a/practice_note.xlsx
+++ b/practice_note.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taewo\bigdata_exam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65093402-97EF-4623-9556-94549B74FCDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1416E7B8-D223-4D88-90C9-B5386D77C937}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5556" xr2:uid="{531C6767-044B-4F45-8E56-A164CE783FA8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>실기과목명</t>
   </si>
@@ -130,6 +130,10 @@
   </si>
   <si>
     <t>prac_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -589,7 +593,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -666,6 +670,9 @@
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="9"/>
@@ -675,6 +682,9 @@
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>